<commit_message>
update eight files in folder lai
</commit_message>
<xml_diff>
--- a/lai/valuationquan/szseinnovation100ETF/szseinnovation100ETFmodel1.xlsx
+++ b/lai/valuationquan/szseinnovation100ETF/szseinnovation100ETFmodel1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-1485" yWindow="480" windowWidth="15600" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="-1485" yWindow="480" windowWidth="15600" windowHeight="7620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="model1" sheetId="4" r:id="rId1"/>
@@ -2356,7 +2356,7 @@
               <c:f>model1!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -2407,6 +2407,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2416,7 +2419,7 @@
               <c:f>model1!资金</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -2467,6 +2470,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>34000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>36000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2509,7 +2515,7 @@
               <c:f>model1!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -2560,6 +2566,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2569,7 +2578,7 @@
               <c:f>model1!资产</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -2620,6 +2629,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>27375.140717758622</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30690.105924803764</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2662,7 +2674,7 @@
               <c:f>model1!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -2713,6 +2725,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2722,7 +2737,7 @@
               <c:f>model1!金额</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2773,6 +2788,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>-6624.8592822413775</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-5309.8940751962364</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2794,11 +2812,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="71011328"/>
-        <c:axId val="91754496"/>
+        <c:axId val="77735424"/>
+        <c:axId val="77736960"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="71011328"/>
+        <c:axId val="77735424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2841,14 +2859,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91754496"/>
+        <c:crossAx val="77736960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="91754496"/>
+        <c:axId val="77736960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2899,7 +2917,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71011328"/>
+        <c:crossAx val="77735424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3066,7 +3084,7 @@
               <c:f>'model1&amp;CCI'!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -3117,6 +3135,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3126,7 +3147,7 @@
               <c:f>'model1&amp;CCI'!资金</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3176,6 +3197,9 @@
                   <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>12000</c:v>
                 </c:pt>
               </c:numCache>
@@ -3219,7 +3243,7 @@
               <c:f>'model1&amp;CCI'!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -3270,6 +3294,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3279,7 +3306,7 @@
               <c:f>'model1&amp;CCI'!资产</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3330,6 +3357,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>10450.019810272373</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10951.986635031977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3372,7 +3402,7 @@
               <c:f>'model1&amp;CCI'!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -3423,6 +3453,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3432,7 +3465,7 @@
               <c:f>'model1&amp;CCI'!金额</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3483,6 +3516,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>-1549.9801897276266</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1048.0133649680229</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3504,11 +3540,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="594687488"/>
-        <c:axId val="594689024"/>
+        <c:axId val="91410432"/>
+        <c:axId val="91412352"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="594687488"/>
+        <c:axId val="91410432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3551,14 +3587,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="594689024"/>
+        <c:crossAx val="91412352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="594689024"/>
+        <c:axId val="91412352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3609,7 +3645,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="594687488"/>
+        <c:crossAx val="91410432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3776,7 +3812,7 @@
               <c:f>'model1&amp;RSI'!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -3827,6 +3863,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3836,7 +3875,7 @@
               <c:f>'model1&amp;RSI'!资金</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -3887,6 +3926,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>42000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3929,7 +3971,7 @@
               <c:f>'model1&amp;RSI'!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -3980,6 +4022,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3989,7 +4034,7 @@
               <c:f>'model1&amp;RSI'!资产</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -4040,6 +4085,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>33776.655628449436</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>37399.117679683528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4082,7 +4130,7 @@
               <c:f>'model1&amp;RSI'!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -4133,6 +4181,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4142,7 +4193,7 @@
               <c:f>'model1&amp;RSI'!金额</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4193,6 +4244,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>-8223.3443715505637</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-6600.882320316472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4214,11 +4268,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="624148864"/>
-        <c:axId val="624150400"/>
+        <c:axId val="535953792"/>
+        <c:axId val="535955712"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="624148864"/>
+        <c:axId val="535953792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4261,14 +4315,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="624150400"/>
+        <c:crossAx val="535955712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="624150400"/>
+        <c:axId val="535955712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4319,7 +4373,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="624148864"/>
+        <c:crossAx val="535953792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4440,7 +4494,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4487,7 +4540,7 @@
               <c:f>'model1&amp;KDJ'!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -4538,6 +4591,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4547,7 +4603,7 @@
               <c:f>'model1&amp;KDJ'!资金</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -4598,6 +4654,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>37000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4640,7 +4699,7 @@
               <c:f>'model1&amp;KDJ'!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -4691,6 +4750,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4700,7 +4762,7 @@
               <c:f>'model1&amp;KDJ'!资产</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -4751,6 +4813,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>28242.564935381801</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>31599.196874944704</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4793,7 +4858,7 @@
               <c:f>'model1&amp;KDJ'!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -4844,6 +4909,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4853,7 +4921,7 @@
               <c:f>'model1&amp;KDJ'!金额</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4904,6 +4972,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>-6757.4350646181992</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-5400.8031250552958</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4925,11 +4996,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="711798144"/>
-        <c:axId val="619009152"/>
+        <c:axId val="567309056"/>
+        <c:axId val="567310592"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="711798144"/>
+        <c:axId val="567309056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4972,14 +5043,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="619009152"/>
+        <c:crossAx val="567310592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="619009152"/>
+        <c:axId val="567310592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5030,7 +5101,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="711798144"/>
+        <c:crossAx val="567309056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5044,7 +5115,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5152,6 +5222,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5198,7 +5269,7 @@
               <c:f>'model1&amp;2'!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -5249,6 +5320,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5258,7 +5332,7 @@
               <c:f>'model1&amp;2'!资金</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -5309,6 +5383,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>34000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>36000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5351,7 +5428,7 @@
               <c:f>'model1&amp;2'!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -5402,6 +5479,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5411,7 +5491,7 @@
               <c:f>'model1&amp;2'!资产</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -5462,6 +5542,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>27375.140717758622</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30690.105924803764</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5504,7 +5587,7 @@
               <c:f>'model1&amp;2'!时间</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44377</c:v>
                 </c:pt>
@@ -5555,6 +5638,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5564,7 +5650,7 @@
               <c:f>'model1&amp;2'!金额</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5615,6 +5701,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>-6624.8592822413775</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-5309.8940751962364</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5636,11 +5725,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="619029248"/>
-        <c:axId val="619030784"/>
+        <c:axId val="69429120"/>
+        <c:axId val="69430656"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="619029248"/>
+        <c:axId val="69429120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5683,14 +5772,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="619030784"/>
+        <c:crossAx val="69430656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="619030784"/>
+        <c:axId val="69430656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5741,7 +5830,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="619029248"/>
+        <c:crossAx val="69429120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5755,6 +5844,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6852,6 +6942,12 @@
           <cell r="I19">
             <v>43642273.117647059</v>
           </cell>
+          <cell r="K19">
+            <v>44925</v>
+          </cell>
+          <cell r="L19">
+            <v>44896</v>
+          </cell>
           <cell r="N19">
             <v>1.0529999999999999</v>
           </cell>
@@ -23230,10 +23326,10 @@
             <v>5444602.8119248468</v>
           </cell>
           <cell r="N328">
-            <v>0</v>
+            <v>0.70499998331069946</v>
           </cell>
           <cell r="O328">
-            <v>0</v>
+            <v>0.68400001525878906</v>
           </cell>
           <cell r="P328">
             <v>0.68566664059956872</v>
@@ -23252,6 +23348,1172 @@
           </cell>
           <cell r="U328">
             <v>-146.0933885866429</v>
+          </cell>
+        </row>
+        <row r="329">
+          <cell r="A329">
+            <v>44866</v>
+          </cell>
+          <cell r="B329">
+            <v>0.68900001049041748</v>
+          </cell>
+          <cell r="C329">
+            <v>0.70499998331069946</v>
+          </cell>
+          <cell r="D329">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="E329">
+            <v>0.70499998331069946</v>
+          </cell>
+          <cell r="F329">
+            <v>4066501.25</v>
+          </cell>
+          <cell r="G329">
+            <v>2806.73095703125</v>
+          </cell>
+          <cell r="H329">
+            <v>327</v>
+          </cell>
+          <cell r="I329">
+            <v>5440388.4340596329</v>
+          </cell>
+          <cell r="N329">
+            <v>0.70499998331069946</v>
+          </cell>
+          <cell r="O329">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P329">
+            <v>0.69799999396006263</v>
+          </cell>
+          <cell r="Q329">
+            <v>0.71021428420430144</v>
+          </cell>
+          <cell r="R329">
+            <v>-1.2214290244238812E-2</v>
+          </cell>
+          <cell r="S329">
+            <v>1.0785711663109923E-2</v>
+          </cell>
+          <cell r="T329">
+            <v>1.6178567494664885E-4</v>
+          </cell>
+          <cell r="U329">
+            <v>-75.496735098868612</v>
+          </cell>
+        </row>
+        <row r="330">
+          <cell r="A330">
+            <v>44867</v>
+          </cell>
+          <cell r="B330">
+            <v>0.70499998331069946</v>
+          </cell>
+          <cell r="C330">
+            <v>0.72200000286102295</v>
+          </cell>
+          <cell r="D330">
+            <v>0.70499998331069946</v>
+          </cell>
+          <cell r="E330">
+            <v>0.71700000762939453</v>
+          </cell>
+          <cell r="F330">
+            <v>3588100</v>
+          </cell>
+          <cell r="G330">
+            <v>2554.7890625</v>
+          </cell>
+          <cell r="H330">
+            <v>328</v>
+          </cell>
+          <cell r="I330">
+            <v>5434741.213224085</v>
+          </cell>
+          <cell r="N330">
+            <v>0.72200000286102295</v>
+          </cell>
+          <cell r="O330">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P330">
+            <v>0.71466666460037231</v>
+          </cell>
+          <cell r="Q330">
+            <v>0.71064285437266039</v>
+          </cell>
+          <cell r="R330">
+            <v>4.0238102277119214E-3</v>
+          </cell>
+          <cell r="S330">
+            <v>1.0931971527281259E-2</v>
+          </cell>
+          <cell r="T330">
+            <v>1.6397957290921887E-4</v>
+          </cell>
+          <cell r="U330">
+            <v>24.538484619297996</v>
+          </cell>
+        </row>
+        <row r="331">
+          <cell r="A331">
+            <v>44868</v>
+          </cell>
+          <cell r="B331">
+            <v>0.71100002527236938</v>
+          </cell>
+          <cell r="C331">
+            <v>0.7149999737739563</v>
+          </cell>
+          <cell r="D331">
+            <v>0.70999997854232788</v>
+          </cell>
+          <cell r="E331">
+            <v>0.71299999952316284</v>
+          </cell>
+          <cell r="F331">
+            <v>2969101</v>
+          </cell>
+          <cell r="G331">
+            <v>2118.14306640625</v>
+          </cell>
+          <cell r="H331">
+            <v>329</v>
+          </cell>
+          <cell r="I331">
+            <v>5427246.8660714282</v>
+          </cell>
+          <cell r="N331">
+            <v>0.72200000286102295</v>
+          </cell>
+          <cell r="O331">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P331">
+            <v>0.71266665061314904</v>
+          </cell>
+          <cell r="Q331">
+            <v>0.71026190121968591</v>
+          </cell>
+          <cell r="R331">
+            <v>2.4047493934631348E-3</v>
+          </cell>
+          <cell r="S331">
+            <v>1.0605440253303169E-2</v>
+          </cell>
+          <cell r="T331">
+            <v>1.5908160379954754E-4</v>
+          </cell>
+          <cell r="U331">
+            <v>15.116451783408374</v>
+          </cell>
+        </row>
+        <row r="332">
+          <cell r="A332">
+            <v>44869</v>
+          </cell>
+          <cell r="B332">
+            <v>0.7160000205039978</v>
+          </cell>
+          <cell r="C332">
+            <v>0.73799997568130493</v>
+          </cell>
+          <cell r="D332">
+            <v>0.7160000205039978</v>
+          </cell>
+          <cell r="E332">
+            <v>0.73600000143051147</v>
+          </cell>
+          <cell r="F332">
+            <v>3661902</v>
+          </cell>
+          <cell r="G332">
+            <v>2657.242919921875</v>
+          </cell>
+          <cell r="H332">
+            <v>330</v>
+          </cell>
+          <cell r="I332">
+            <v>5421897.3361742422</v>
+          </cell>
+          <cell r="N332">
+            <v>0.73799997568130493</v>
+          </cell>
+          <cell r="O332">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P332">
+            <v>0.72999999920527137</v>
+          </cell>
+          <cell r="Q332">
+            <v>0.71057142530168804</v>
+          </cell>
+          <cell r="R332">
+            <v>1.9428573903583324E-2</v>
+          </cell>
+          <cell r="S332">
+            <v>1.0870746609305046E-2</v>
+          </cell>
+          <cell r="T332">
+            <v>1.630611991395757E-4</v>
+          </cell>
+          <cell r="U332">
+            <v>119.14896987206026</v>
+          </cell>
+        </row>
+        <row r="333">
+          <cell r="A333">
+            <v>44872</v>
+          </cell>
+          <cell r="B333">
+            <v>0.73500001430511475</v>
+          </cell>
+          <cell r="C333">
+            <v>0.73900002241134644</v>
+          </cell>
+          <cell r="D333">
+            <v>0.73100000619888306</v>
+          </cell>
+          <cell r="E333">
+            <v>0.73400002717971802</v>
+          </cell>
+          <cell r="F333">
+            <v>2424500</v>
+          </cell>
+          <cell r="G333">
+            <v>1782.22900390625</v>
+          </cell>
+          <cell r="H333">
+            <v>331</v>
+          </cell>
+          <cell r="I333">
+            <v>5412841.7550981874</v>
+          </cell>
+          <cell r="N333">
+            <v>0.73900002241134644</v>
+          </cell>
+          <cell r="O333">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P333">
+            <v>0.7346666852633158</v>
+          </cell>
+          <cell r="Q333">
+            <v>0.71064285579181852</v>
+          </cell>
+          <cell r="R333">
+            <v>2.4023829471497282E-2</v>
+          </cell>
+          <cell r="S333">
+            <v>1.0931972743702587E-2</v>
+          </cell>
+          <cell r="T333">
+            <v>1.639795911555388E-4</v>
+          </cell>
+          <cell r="U333">
+            <v>146.50499676334766</v>
+          </cell>
+        </row>
+        <row r="334">
+          <cell r="A334">
+            <v>44873</v>
+          </cell>
+          <cell r="B334">
+            <v>0.73600000143051147</v>
+          </cell>
+          <cell r="C334">
+            <v>0.73600000143051147</v>
+          </cell>
+          <cell r="D334">
+            <v>0.72399997711181641</v>
+          </cell>
+          <cell r="E334">
+            <v>0.72699999809265137</v>
+          </cell>
+          <cell r="F334">
+            <v>2755801</v>
+          </cell>
+          <cell r="G334">
+            <v>2007.2960205078125</v>
+          </cell>
+          <cell r="H334">
+            <v>332</v>
+          </cell>
+          <cell r="I334">
+            <v>5404838.620293675</v>
+          </cell>
+          <cell r="N334">
+            <v>0.73900002241134644</v>
+          </cell>
+          <cell r="O334">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P334">
+            <v>0.72899999221165979</v>
+          </cell>
+          <cell r="Q334">
+            <v>0.71076190329733346</v>
+          </cell>
+          <cell r="R334">
+            <v>1.8238088914326323E-2</v>
+          </cell>
+          <cell r="S334">
+            <v>1.1034013462715415E-2</v>
+          </cell>
+          <cell r="T334">
+            <v>1.6551020194073123E-4</v>
+          </cell>
+          <cell r="U334">
+            <v>110.19314036519232</v>
+          </cell>
+        </row>
+        <row r="335">
+          <cell r="A335">
+            <v>44874</v>
+          </cell>
+          <cell r="B335">
+            <v>0.73000001907348633</v>
+          </cell>
+          <cell r="C335">
+            <v>0.73000001907348633</v>
+          </cell>
+          <cell r="D335">
+            <v>0.72100001573562622</v>
+          </cell>
+          <cell r="E335">
+            <v>0.72200000286102295</v>
+          </cell>
+          <cell r="F335">
+            <v>2908406</v>
+          </cell>
+          <cell r="G335">
+            <v>2104.299072265625</v>
+          </cell>
+          <cell r="H335">
+            <v>333</v>
+          </cell>
+          <cell r="I335">
+            <v>5397341.8256381378</v>
+          </cell>
+          <cell r="N335">
+            <v>0.73900002241134644</v>
+          </cell>
+          <cell r="O335">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P335">
+            <v>0.72433334589004517</v>
+          </cell>
+          <cell r="Q335">
+            <v>0.71130952380952384</v>
+          </cell>
+          <cell r="R335">
+            <v>1.302382208052133E-2</v>
+          </cell>
+          <cell r="S335">
+            <v>1.1547619388217023E-2</v>
+          </cell>
+          <cell r="T335">
+            <v>1.7321429082325533E-4</v>
+          </cell>
+          <cell r="U335">
+            <v>75.189073711075025</v>
+          </cell>
+        </row>
+        <row r="336">
+          <cell r="A336">
+            <v>44875</v>
+          </cell>
+          <cell r="B336">
+            <v>0.72000002861022949</v>
+          </cell>
+          <cell r="C336">
+            <v>0.72000002861022949</v>
+          </cell>
+          <cell r="D336">
+            <v>0.70499998331069946</v>
+          </cell>
+          <cell r="E336">
+            <v>0.70899999141693115</v>
+          </cell>
+          <cell r="F336">
+            <v>3683300</v>
+          </cell>
+          <cell r="G336">
+            <v>2612.735107421875</v>
+          </cell>
+          <cell r="H336">
+            <v>334</v>
+          </cell>
+          <cell r="I336">
+            <v>5392209.9638847308</v>
+          </cell>
+          <cell r="N336">
+            <v>0.73900002241134644</v>
+          </cell>
+          <cell r="O336">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P336">
+            <v>0.71133333444595337</v>
+          </cell>
+          <cell r="Q336">
+            <v>0.71107142879849394</v>
+          </cell>
+          <cell r="R336">
+            <v>2.6190564745942613E-4</v>
+          </cell>
+          <cell r="S336">
+            <v>1.1309524377187099E-2</v>
+          </cell>
+          <cell r="T336">
+            <v>1.6964286565780646E-4</v>
+          </cell>
+          <cell r="U336">
+            <v>1.5438647917427113</v>
+          </cell>
+        </row>
+        <row r="337">
+          <cell r="A337">
+            <v>44876</v>
+          </cell>
+          <cell r="B337">
+            <v>0.72000002861022949</v>
+          </cell>
+          <cell r="C337">
+            <v>0.73400002717971802</v>
+          </cell>
+          <cell r="D337">
+            <v>0.72000002861022949</v>
+          </cell>
+          <cell r="E337">
+            <v>0.72600001096725464</v>
+          </cell>
+          <cell r="F337">
+            <v>3560304</v>
+          </cell>
+          <cell r="G337">
+            <v>2588.037109375</v>
+          </cell>
+          <cell r="H337">
+            <v>335</v>
+          </cell>
+          <cell r="I337">
+            <v>5386741.5878731348</v>
+          </cell>
+          <cell r="N337">
+            <v>0.73900002241134644</v>
+          </cell>
+          <cell r="O337">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P337">
+            <v>0.72666668891906738</v>
+          </cell>
+          <cell r="Q337">
+            <v>0.71250000170298988</v>
+          </cell>
+          <cell r="R337">
+            <v>1.41666872160775E-2</v>
+          </cell>
+          <cell r="S337">
+            <v>1.2071430683135995E-2</v>
+          </cell>
+          <cell r="T337">
+            <v>1.8107146024703993E-4</v>
+          </cell>
+          <cell r="U337">
+            <v>78.238101116264076</v>
+          </cell>
+        </row>
+        <row r="338">
+          <cell r="A338">
+            <v>44879</v>
+          </cell>
+          <cell r="B338">
+            <v>0.73400002717971802</v>
+          </cell>
+          <cell r="C338">
+            <v>0.73400002717971802</v>
+          </cell>
+          <cell r="D338">
+            <v>0.72100001573562622</v>
+          </cell>
+          <cell r="E338">
+            <v>0.72399997711181641</v>
+          </cell>
+          <cell r="F338">
+            <v>3003903</v>
+          </cell>
+          <cell r="G338">
+            <v>2189.81298828125</v>
+          </cell>
+          <cell r="H338">
+            <v>336</v>
+          </cell>
+          <cell r="I338">
+            <v>5379649.8063616073</v>
+          </cell>
+          <cell r="N338">
+            <v>0.73900002241134644</v>
+          </cell>
+          <cell r="O338">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P338">
+            <v>0.72633334000905359</v>
+          </cell>
+          <cell r="Q338">
+            <v>0.71447619228135972</v>
+          </cell>
+          <cell r="R338">
+            <v>1.1857147727693862E-2</v>
+          </cell>
+          <cell r="S338">
+            <v>1.2047624304181057E-2</v>
+          </cell>
+          <cell r="T338">
+            <v>1.8071436456271585E-4</v>
+          </cell>
+          <cell r="U338">
+            <v>65.612646545199837</v>
+          </cell>
+        </row>
+        <row r="339">
+          <cell r="A339">
+            <v>44880</v>
+          </cell>
+          <cell r="B339">
+            <v>0.72500002384185791</v>
+          </cell>
+          <cell r="C339">
+            <v>0.74299997091293335</v>
+          </cell>
+          <cell r="D339">
+            <v>0.72200000286102295</v>
+          </cell>
+          <cell r="E339">
+            <v>0.74299997091293335</v>
+          </cell>
+          <cell r="F339">
+            <v>5722604</v>
+          </cell>
+          <cell r="G339">
+            <v>4205.744140625</v>
+          </cell>
+          <cell r="H339">
+            <v>337</v>
+          </cell>
+          <cell r="I339">
+            <v>5380667.4745919881</v>
+          </cell>
+          <cell r="N339">
+            <v>0.74299997091293335</v>
+          </cell>
+          <cell r="O339">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P339">
+            <v>0.73599998156229651</v>
+          </cell>
+          <cell r="Q339">
+            <v>0.71626190486408425</v>
+          </cell>
+          <cell r="R339">
+            <v>1.9738076698212259E-2</v>
+          </cell>
+          <cell r="S339">
+            <v>1.3309528430302935E-2</v>
+          </cell>
+          <cell r="T339">
+            <v>1.9964292645454401E-4</v>
+          </cell>
+          <cell r="U339">
+            <v>98.866897258723327</v>
+          </cell>
+        </row>
+        <row r="340">
+          <cell r="A340">
+            <v>44881</v>
+          </cell>
+          <cell r="B340">
+            <v>0.74299997091293335</v>
+          </cell>
+          <cell r="C340">
+            <v>0.74500000476837158</v>
+          </cell>
+          <cell r="D340">
+            <v>0.73400002717971802</v>
+          </cell>
+          <cell r="E340">
+            <v>0.73400002717971802</v>
+          </cell>
+          <cell r="F340">
+            <v>1012900</v>
+          </cell>
+          <cell r="G340">
+            <v>748.44000244140625</v>
+          </cell>
+          <cell r="H340">
+            <v>338</v>
+          </cell>
+          <cell r="I340">
+            <v>5367745.0856139055</v>
+          </cell>
+          <cell r="N340">
+            <v>0.74500000476837158</v>
+          </cell>
+          <cell r="O340">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P340">
+            <v>0.73766668637593591</v>
+          </cell>
+          <cell r="Q340">
+            <v>0.71826190607888363</v>
+          </cell>
+          <cell r="R340">
+            <v>1.9404780297052282E-2</v>
+          </cell>
+          <cell r="S340">
+            <v>1.4081638686510975E-2</v>
+          </cell>
+          <cell r="T340">
+            <v>2.1122458029766461E-4</v>
+          </cell>
+          <cell r="U340">
+            <v>91.868002624062171</v>
+          </cell>
+        </row>
+        <row r="341">
+          <cell r="A341">
+            <v>44882</v>
+          </cell>
+          <cell r="B341">
+            <v>0.73100000619888306</v>
+          </cell>
+          <cell r="C341">
+            <v>0.73100000619888306</v>
+          </cell>
+          <cell r="D341">
+            <v>0.72100001573562622</v>
+          </cell>
+          <cell r="E341">
+            <v>0.73000001907348633</v>
+          </cell>
+          <cell r="F341">
+            <v>3281900</v>
+          </cell>
+          <cell r="G341">
+            <v>2381.821044921875</v>
+          </cell>
+          <cell r="H341">
+            <v>339</v>
+          </cell>
+          <cell r="I341">
+            <v>5361592.1502581118</v>
+          </cell>
+          <cell r="N341">
+            <v>0.74500000476837158</v>
+          </cell>
+          <cell r="O341">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P341">
+            <v>0.72733334700266516</v>
+          </cell>
+          <cell r="Q341">
+            <v>0.7210238107613155</v>
+          </cell>
+          <cell r="R341">
+            <v>6.309536241349667E-3</v>
+          </cell>
+          <cell r="S341">
+            <v>1.1826538512495901E-2</v>
+          </cell>
+          <cell r="T341">
+            <v>1.7739807768743851E-4</v>
+          </cell>
+          <cell r="U341">
+            <v>35.567106045346073</v>
+          </cell>
+        </row>
+        <row r="342">
+          <cell r="A342">
+            <v>44883</v>
+          </cell>
+          <cell r="B342">
+            <v>0.73100000619888306</v>
+          </cell>
+          <cell r="C342">
+            <v>0.73900002241134644</v>
+          </cell>
+          <cell r="D342">
+            <v>0.73100000619888306</v>
+          </cell>
+          <cell r="E342">
+            <v>0.73100000619888306</v>
+          </cell>
+          <cell r="F342">
+            <v>2393401</v>
+          </cell>
+          <cell r="G342">
+            <v>1758.56494140625</v>
+          </cell>
+          <cell r="H342">
+            <v>340</v>
+          </cell>
+          <cell r="I342">
+            <v>5352862.1762867644</v>
+          </cell>
+          <cell r="N342">
+            <v>0.74500000476837158</v>
+          </cell>
+          <cell r="O342">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P342">
+            <v>0.73366667826970422</v>
+          </cell>
+          <cell r="Q342">
+            <v>0.72445238488061092</v>
+          </cell>
+          <cell r="R342">
+            <v>9.2142933890932976E-3</v>
+          </cell>
+          <cell r="S342">
+            <v>8.7517049847816806E-3</v>
+          </cell>
+          <cell r="T342">
+            <v>1.312755747717252E-4</v>
+          </cell>
+          <cell r="U342">
+            <v>70.190463116356653</v>
+          </cell>
+        </row>
+        <row r="343">
+          <cell r="A343">
+            <v>44886</v>
+          </cell>
+          <cell r="B343">
+            <v>0.72899997234344482</v>
+          </cell>
+          <cell r="C343">
+            <v>0.72899997234344482</v>
+          </cell>
+          <cell r="D343">
+            <v>0.72100001573562622</v>
+          </cell>
+          <cell r="E343">
+            <v>0.72899997234344482</v>
+          </cell>
+          <cell r="F343">
+            <v>3153102</v>
+          </cell>
+          <cell r="G343">
+            <v>2289.886962890625</v>
+          </cell>
+          <cell r="H343">
+            <v>341</v>
+          </cell>
+          <cell r="I343">
+            <v>5346411.2666788856</v>
+          </cell>
+          <cell r="N343">
+            <v>0.74500000476837158</v>
+          </cell>
+          <cell r="O343">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P343">
+            <v>0.72633332014083862</v>
+          </cell>
+          <cell r="Q343">
+            <v>0.72647619389352347</v>
+          </cell>
+          <cell r="R343">
+            <v>-1.428737526848467E-4</v>
+          </cell>
+          <cell r="S343">
+            <v>6.1700725231040787E-3</v>
+          </cell>
+          <cell r="T343">
+            <v>9.2551087846561177E-5</v>
+          </cell>
+          <cell r="U343">
+            <v>-1.5437285072403966</v>
+          </cell>
+        </row>
+        <row r="344">
+          <cell r="A344">
+            <v>44887</v>
+          </cell>
+          <cell r="B344">
+            <v>0.72299998998641968</v>
+          </cell>
+          <cell r="C344">
+            <v>0.72399997711181641</v>
+          </cell>
+          <cell r="D344">
+            <v>0.7160000205039978</v>
+          </cell>
+          <cell r="E344">
+            <v>0.7160000205039978</v>
+          </cell>
+          <cell r="F344">
+            <v>3219613</v>
+          </cell>
+          <cell r="G344">
+            <v>2322.748046875</v>
+          </cell>
+          <cell r="H344">
+            <v>342</v>
+          </cell>
+          <cell r="I344">
+            <v>5340192.5582967838</v>
+          </cell>
+          <cell r="N344">
+            <v>0.74500000476837158</v>
+          </cell>
+          <cell r="O344">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P344">
+            <v>0.718666672706604</v>
+          </cell>
+          <cell r="Q344">
+            <v>0.7267619087582543</v>
+          </cell>
+          <cell r="R344">
+            <v>-8.0952360516503008E-3</v>
+          </cell>
+          <cell r="S344">
+            <v>5.8571440832955414E-3</v>
+          </cell>
+          <cell r="T344">
+            <v>8.7857161249433113E-5</v>
+          </cell>
+          <cell r="U344">
+            <v>-92.140878859804204</v>
+          </cell>
+        </row>
+        <row r="345">
+          <cell r="A345">
+            <v>44888</v>
+          </cell>
+          <cell r="B345">
+            <v>0.7160000205039978</v>
+          </cell>
+          <cell r="C345">
+            <v>0.71899998188018799</v>
+          </cell>
+          <cell r="D345">
+            <v>0.71100002527236938</v>
+          </cell>
+          <cell r="E345">
+            <v>0.71700000762939453</v>
+          </cell>
+          <cell r="F345">
+            <v>2462800</v>
+          </cell>
+          <cell r="G345">
+            <v>1759.5560302734375</v>
+          </cell>
+          <cell r="H345">
+            <v>343</v>
+          </cell>
+          <cell r="I345">
+            <v>5331803.6587099126</v>
+          </cell>
+          <cell r="N345">
+            <v>0.74500000476837158</v>
+          </cell>
+          <cell r="O345">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P345">
+            <v>0.71566667159398401</v>
+          </cell>
+          <cell r="Q345">
+            <v>0.72697619597117114</v>
+          </cell>
+          <cell r="R345">
+            <v>-1.130952437718713E-2</v>
+          </cell>
+          <cell r="S345">
+            <v>5.6428568703787586E-3</v>
+          </cell>
+          <cell r="T345">
+            <v>8.4642853055681371E-5</v>
+          </cell>
+          <cell r="U345">
+            <v>-133.61464044397562</v>
+          </cell>
+        </row>
+        <row r="346">
+          <cell r="A346">
+            <v>44889</v>
+          </cell>
+          <cell r="B346">
+            <v>0.72000002861022949</v>
+          </cell>
+          <cell r="C346">
+            <v>0.72000002861022949</v>
+          </cell>
+          <cell r="D346">
+            <v>0.71299999952316284</v>
+          </cell>
+          <cell r="E346">
+            <v>0.71399998664855957</v>
+          </cell>
+          <cell r="F346">
+            <v>2647100</v>
+          </cell>
+          <cell r="G346">
+            <v>1893.616943359375</v>
+          </cell>
+          <cell r="H346">
+            <v>344</v>
+          </cell>
+          <cell r="I346">
+            <v>5323999.2876090119</v>
+          </cell>
+          <cell r="N346">
+            <v>0.74500000476837158</v>
+          </cell>
+          <cell r="O346">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P346">
+            <v>0.71566667159398401</v>
+          </cell>
+          <cell r="Q346">
+            <v>0.7259523868560791</v>
+          </cell>
+          <cell r="R346">
+            <v>-1.0285715262095096E-2</v>
+          </cell>
+          <cell r="S346">
+            <v>6.2993197214035734E-3</v>
+          </cell>
+          <cell r="T346">
+            <v>9.4489795821053597E-5</v>
+          </cell>
+          <cell r="U346">
+            <v>-108.8553020219703</v>
+          </cell>
+        </row>
+        <row r="347">
+          <cell r="A347">
+            <v>44890</v>
+          </cell>
+          <cell r="B347">
+            <v>0.7070000171661377</v>
+          </cell>
+          <cell r="C347">
+            <v>0.72000002861022949</v>
+          </cell>
+          <cell r="D347">
+            <v>0.7070000171661377</v>
+          </cell>
+          <cell r="E347">
+            <v>0.70899999141693115</v>
+          </cell>
+          <cell r="F347">
+            <v>1362800</v>
+          </cell>
+          <cell r="G347">
+            <v>968.49102783203125</v>
+          </cell>
+          <cell r="H347">
+            <v>345</v>
+          </cell>
+          <cell r="I347">
+            <v>5312517.5505434787</v>
+          </cell>
+          <cell r="N347">
+            <v>0.74500000476837158</v>
+          </cell>
+          <cell r="O347">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P347">
+            <v>0.71200001239776611</v>
+          </cell>
+          <cell r="Q347">
+            <v>0.72433333879425421</v>
+          </cell>
+          <cell r="R347">
+            <v>-1.2333326396488098E-2</v>
+          </cell>
+          <cell r="S347">
+            <v>6.904761604711286E-3</v>
+          </cell>
+          <cell r="T347">
+            <v>1.0357142407066929E-4</v>
+          </cell>
+          <cell r="U347">
+            <v>-119.08039796838915</v>
+          </cell>
+        </row>
+        <row r="348">
+          <cell r="A348">
+            <v>44893</v>
+          </cell>
+          <cell r="B348">
+            <v>0.70999997854232788</v>
+          </cell>
+          <cell r="C348">
+            <v>0.70999997854232788</v>
+          </cell>
+          <cell r="D348">
+            <v>0.6940000057220459</v>
+          </cell>
+          <cell r="E348">
+            <v>0.70499998331069946</v>
+          </cell>
+          <cell r="F348">
+            <v>2657600</v>
+          </cell>
+          <cell r="G348">
+            <v>1855.81494140625</v>
+          </cell>
+          <cell r="H348">
+            <v>346</v>
+          </cell>
+          <cell r="I348">
+            <v>5304844.3784320811</v>
+          </cell>
+          <cell r="N348">
+            <v>0.74500000476837158</v>
+          </cell>
+          <cell r="O348">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P348">
+            <v>0.70299998919169104</v>
+          </cell>
+          <cell r="Q348">
+            <v>0.72247619572139921</v>
+          </cell>
+          <cell r="R348">
+            <v>-1.9476206529708162E-2</v>
+          </cell>
+          <cell r="S348">
+            <v>8.3605460569161159E-3</v>
+          </cell>
+          <cell r="T348">
+            <v>1.2540819085374172E-4</v>
+          </cell>
+          <cell r="U348">
+            <v>-155.30250773191074</v>
+          </cell>
+        </row>
+        <row r="349">
+          <cell r="A349">
+            <v>44894</v>
+          </cell>
+          <cell r="B349">
+            <v>0.70899999141693115</v>
+          </cell>
+          <cell r="C349">
+            <v>0.72000002861022949</v>
+          </cell>
+          <cell r="D349">
+            <v>0.70800000429153442</v>
+          </cell>
+          <cell r="E349">
+            <v>0.71899998188018799</v>
+          </cell>
+          <cell r="F349">
+            <v>2146700</v>
+          </cell>
+          <cell r="G349">
+            <v>1530.8990478515625</v>
+          </cell>
+          <cell r="H349">
+            <v>347</v>
+          </cell>
+          <cell r="I349">
+            <v>5295743.0978025934</v>
+          </cell>
+          <cell r="N349">
+            <v>0.74500000476837158</v>
+          </cell>
+          <cell r="O349">
+            <v>0.68400001525878906</v>
+          </cell>
+          <cell r="P349">
+            <v>0.71566667159398401</v>
+          </cell>
+          <cell r="Q349">
+            <v>0.72185714755739483</v>
+          </cell>
+          <cell r="R349">
+            <v>-6.1904759634108242E-3</v>
+          </cell>
+          <cell r="S349">
+            <v>8.7142870539710614E-3</v>
+          </cell>
+          <cell r="T349">
+            <v>1.3071430580956591E-4</v>
+          </cell>
+          <cell r="U349">
+            <v>-47.358825226288232</v>
+          </cell>
+        </row>
+        <row r="350">
+          <cell r="A350">
+            <v>44895</v>
+          </cell>
+          <cell r="B350">
+            <v>0.71899998188018799</v>
+          </cell>
+          <cell r="C350">
+            <v>0.72399997711181641</v>
+          </cell>
+          <cell r="D350">
+            <v>0.71899998188018799</v>
+          </cell>
+          <cell r="E350">
+            <v>0.72000002861022949</v>
+          </cell>
+          <cell r="F350">
+            <v>2516800</v>
+          </cell>
+          <cell r="G350">
+            <v>1814.135986328125</v>
+          </cell>
+          <cell r="H350">
+            <v>348</v>
+          </cell>
+          <cell r="I350">
+            <v>5287757.6291307472</v>
+          </cell>
+          <cell r="N350">
+            <v>0</v>
+          </cell>
+          <cell r="O350">
+            <v>0</v>
+          </cell>
+          <cell r="P350">
+            <v>0.72099999586741126</v>
+          </cell>
+          <cell r="Q350">
+            <v>0.72254762337321321</v>
+          </cell>
+          <cell r="R350">
+            <v>-1.5476275058019517E-3</v>
+          </cell>
+          <cell r="S350">
+            <v>8.0238112381526405E-3</v>
+          </cell>
+          <cell r="T350">
+            <v>1.203571685722896E-4</v>
+          </cell>
+          <cell r="U350">
+            <v>-12.858623413630797</v>
           </cell>
         </row>
       </sheetData>
@@ -26545,6 +27807,203 @@
           </cell>
           <cell r="C383">
             <v>22.239999770000001</v>
+          </cell>
+        </row>
+        <row r="384">
+          <cell r="B384" t="str">
+            <v xml:space="preserve">2022/11/1
+</v>
+          </cell>
+          <cell r="C384">
+            <v>22.270000459999999</v>
+          </cell>
+        </row>
+        <row r="385">
+          <cell r="B385" t="str">
+            <v xml:space="preserve">2022/11/2
+</v>
+          </cell>
+          <cell r="C385">
+            <v>22.600000380000001</v>
+          </cell>
+        </row>
+        <row r="386">
+          <cell r="B386" t="str">
+            <v xml:space="preserve">2022/11/3
+</v>
+          </cell>
+          <cell r="C386">
+            <v>22.479999540000001</v>
+          </cell>
+        </row>
+        <row r="387">
+          <cell r="B387" t="str">
+            <v xml:space="preserve">2022/11/4
+</v>
+          </cell>
+          <cell r="C387">
+            <v>23.200000760000002</v>
+          </cell>
+        </row>
+        <row r="388">
+          <cell r="B388" t="str">
+            <v xml:space="preserve">2022/11/7
+</v>
+          </cell>
+          <cell r="C388">
+            <v>23.190000529999999</v>
+          </cell>
+        </row>
+        <row r="389">
+          <cell r="B389" t="str">
+            <v xml:space="preserve">2022/11/8
+</v>
+          </cell>
+          <cell r="C389">
+            <v>23.030000690000001</v>
+          </cell>
+        </row>
+        <row r="390">
+          <cell r="B390" t="str">
+            <v xml:space="preserve">2022/11/9
+</v>
+          </cell>
+          <cell r="C390">
+            <v>22.760000229999999</v>
+          </cell>
+        </row>
+        <row r="391">
+          <cell r="B391" t="str">
+            <v xml:space="preserve">2022/11/10
+</v>
+          </cell>
+          <cell r="C391">
+            <v>22.31999969</v>
+          </cell>
+        </row>
+        <row r="392">
+          <cell r="B392" t="str">
+            <v xml:space="preserve">2022/11/11
+</v>
+          </cell>
+          <cell r="C392">
+            <v>22.870000839999999</v>
+          </cell>
+        </row>
+        <row r="393">
+          <cell r="B393" t="str">
+            <v xml:space="preserve">2022/11/14
+</v>
+          </cell>
+          <cell r="C393">
+            <v>22.88999939</v>
+          </cell>
+        </row>
+        <row r="394">
+          <cell r="B394" t="str">
+            <v xml:space="preserve">2022/11/15
+</v>
+          </cell>
+          <cell r="C394">
+            <v>23.450000760000002</v>
+          </cell>
+        </row>
+        <row r="395">
+          <cell r="B395" t="str">
+            <v xml:space="preserve">2022/11/16
+</v>
+          </cell>
+          <cell r="C395">
+            <v>23.129999160000001</v>
+          </cell>
+        </row>
+        <row r="396">
+          <cell r="B396" t="str">
+            <v xml:space="preserve">2022/11/17
+</v>
+          </cell>
+          <cell r="C396">
+            <v>23.010000229999999</v>
+          </cell>
+        </row>
+        <row r="397">
+          <cell r="B397" t="str">
+            <v xml:space="preserve">2022/11/18
+</v>
+          </cell>
+          <cell r="C397">
+            <v>23.030000690000001</v>
+          </cell>
+        </row>
+        <row r="398">
+          <cell r="B398" t="str">
+            <v xml:space="preserve">2022/11/21
+</v>
+          </cell>
+          <cell r="C398">
+            <v>23</v>
+          </cell>
+        </row>
+        <row r="399">
+          <cell r="B399" t="str">
+            <v xml:space="preserve">2022/11/22
+</v>
+          </cell>
+          <cell r="C399">
+            <v>22.649999619999999</v>
+          </cell>
+        </row>
+        <row r="400">
+          <cell r="B400" t="str">
+            <v xml:space="preserve">2022/11/23
+</v>
+          </cell>
+          <cell r="C400">
+            <v>22.540000920000001</v>
+          </cell>
+        </row>
+        <row r="401">
+          <cell r="B401" t="str">
+            <v xml:space="preserve">2022/11/24
+</v>
+          </cell>
+          <cell r="C401">
+            <v>22.510000229999999</v>
+          </cell>
+        </row>
+        <row r="402">
+          <cell r="B402" t="str">
+            <v xml:space="preserve">2022/11/25
+</v>
+          </cell>
+          <cell r="C402">
+            <v>22.36000061</v>
+          </cell>
+        </row>
+        <row r="403">
+          <cell r="B403" t="str">
+            <v xml:space="preserve">2022/11/28
+</v>
+          </cell>
+          <cell r="C403">
+            <v>22.200000760000002</v>
+          </cell>
+        </row>
+        <row r="404">
+          <cell r="B404" t="str">
+            <v xml:space="preserve">2022/11/29
+</v>
+          </cell>
+          <cell r="C404">
+            <v>22.700000760000002</v>
+          </cell>
+        </row>
+        <row r="405">
+          <cell r="B405">
+            <v>44895</v>
+          </cell>
+          <cell r="C405">
+            <v>22.809999470000001</v>
           </cell>
         </row>
       </sheetData>
@@ -26841,7 +28300,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AC19"/>
+  <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -26935,7 +28394,7 @@
         <v>2000</v>
       </c>
       <c r="D3" s="19">
-        <f t="shared" ref="D3:D19" si="0">C3/B3</f>
+        <f t="shared" ref="D3:D20" si="0">C3/B3</f>
         <v>1939.8642095053349</v>
       </c>
       <c r="E3" s="19">
@@ -26943,7 +28402,7 @@
         <v>1939.8642095053349</v>
       </c>
       <c r="F3" s="19">
-        <f t="shared" ref="F3:F19" si="1">E3*B3</f>
+        <f t="shared" ref="F3:F20" si="1">E3*B3</f>
         <v>2000</v>
       </c>
       <c r="G3" s="19">
@@ -26951,11 +28410,11 @@
         <v>2000</v>
       </c>
       <c r="H3" s="19">
-        <f t="shared" ref="H3:H19" si="2">F3</f>
+        <f t="shared" ref="H3:H20" si="2">F3</f>
         <v>2000</v>
       </c>
       <c r="I3" s="19">
-        <f t="shared" ref="I3:I19" si="3">H3-G3</f>
+        <f t="shared" ref="I3:I20" si="3">H3-G3</f>
         <v>0</v>
       </c>
       <c r="J3" s="7"/>
@@ -26999,7 +28458,7 @@
         <v>1.006</v>
       </c>
       <c r="C4" s="18">
-        <f t="shared" ref="C4:C19" si="4">C3</f>
+        <f t="shared" ref="C4:C20" si="4">C3</f>
         <v>2000</v>
       </c>
       <c r="D4" s="19">
@@ -27007,7 +28466,7 @@
         <v>1988.0715705765408</v>
       </c>
       <c r="E4" s="19">
-        <f t="shared" ref="E4:E19" si="5">E3+D4</f>
+        <f t="shared" ref="E4:E20" si="5">E3+D4</f>
         <v>3927.9357800818757</v>
       </c>
       <c r="F4" s="19">
@@ -27015,7 +28474,7 @@
         <v>3951.503394762367</v>
       </c>
       <c r="G4" s="19">
-        <f t="shared" ref="G4:G19" si="6">G3+C4</f>
+        <f t="shared" ref="G4:G20" si="6">G3+C4</f>
         <v>4000</v>
       </c>
       <c r="H4" s="19">
@@ -27657,6 +29116,43 @@
         <v>-6624.8592822413775</v>
       </c>
     </row>
+    <row r="20" spans="1:10" ht="12.75">
+      <c r="A20" s="16">
+        <v>44895</v>
+      </c>
+      <c r="B20" s="17">
+        <f>VLOOKUP(A20,[1]HwabaoWP_szse_innovation_100!$A:$E,5)</f>
+        <v>0.72000002861022949</v>
+      </c>
+      <c r="C20" s="18">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="D20" s="19">
+        <f t="shared" si="0"/>
+        <v>2777.7776673988105</v>
+      </c>
+      <c r="E20" s="19">
+        <f t="shared" si="5"/>
+        <v>42625.145424011906</v>
+      </c>
+      <c r="F20" s="19">
+        <f t="shared" si="1"/>
+        <v>30690.105924803764</v>
+      </c>
+      <c r="G20" s="19">
+        <f t="shared" si="6"/>
+        <v>36000</v>
+      </c>
+      <c r="H20" s="19">
+        <f t="shared" si="2"/>
+        <v>30690.105924803764</v>
+      </c>
+      <c r="I20" s="19">
+        <f t="shared" si="3"/>
+        <v>-5309.8940751962364</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27668,7 +29164,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:AC19"/>
+  <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -27760,11 +29256,11 @@
         <v>1.0309999999999999</v>
       </c>
       <c r="C3" s="18">
-        <f t="shared" ref="C3:C19" si="0">IF(J3&lt;-100,2000,0)</f>
+        <f t="shared" ref="C3:C20" si="0">IF(J3&lt;-100,2000,0)</f>
         <v>0</v>
       </c>
       <c r="D3" s="19">
-        <f t="shared" ref="D3:D19" si="1">C3/B3</f>
+        <f t="shared" ref="D3:D20" si="1">C3/B3</f>
         <v>0</v>
       </c>
       <c r="E3" s="19">
@@ -27772,7 +29268,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="19">
-        <f t="shared" ref="F3:F19" si="2">E3*B3</f>
+        <f t="shared" ref="F3:F20" si="2">E3*B3</f>
         <v>0</v>
       </c>
       <c r="G3" s="19">
@@ -27780,11 +29276,11 @@
         <v>0</v>
       </c>
       <c r="H3" s="19">
-        <f t="shared" ref="H3:H19" si="3">F3</f>
+        <f t="shared" ref="H3:H20" si="3">F3</f>
         <v>0</v>
       </c>
       <c r="I3" s="19">
-        <f t="shared" ref="I3:I19" si="4">H3-G3</f>
+        <f t="shared" ref="I3:I20" si="4">H3-G3</f>
         <v>0</v>
       </c>
       <c r="J3" s="7">
@@ -27839,7 +29335,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="19">
-        <f t="shared" ref="E4:E19" si="5">E3+D4</f>
+        <f t="shared" ref="E4:E20" si="5">E3+D4</f>
         <v>0</v>
       </c>
       <c r="F4" s="19">
@@ -27847,7 +29343,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="19">
-        <f t="shared" ref="G4:G19" si="6">G3+C4</f>
+        <f t="shared" ref="G4:G20" si="6">G3+C4</f>
         <v>0</v>
       </c>
       <c r="H4" s="19">
@@ -28538,6 +30034,47 @@
         <v>-146.0933885866429</v>
       </c>
     </row>
+    <row r="20" spans="1:10" ht="12.75">
+      <c r="A20" s="16">
+        <v>44895</v>
+      </c>
+      <c r="B20" s="17">
+        <f>VLOOKUP(A20,[1]HwabaoWP_szse_innovation_100!$A:$E,5)</f>
+        <v>0.72000002861022949</v>
+      </c>
+      <c r="C20" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="19">
+        <f t="shared" si="5"/>
+        <v>15211.091944221036</v>
+      </c>
+      <c r="F20" s="19">
+        <f t="shared" si="2"/>
+        <v>10951.986635031977</v>
+      </c>
+      <c r="G20" s="19">
+        <f t="shared" si="6"/>
+        <v>12000</v>
+      </c>
+      <c r="H20" s="19">
+        <f t="shared" si="3"/>
+        <v>10951.986635031977</v>
+      </c>
+      <c r="I20" s="19">
+        <f t="shared" si="4"/>
+        <v>-1048.0133649680229</v>
+      </c>
+      <c r="J20" s="7">
+        <f>VLOOKUP(A20,[1]HwabaoWP_szse_innovation_100!$A:$U,21)</f>
+        <v>-12.858623413630797</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28549,7 +30086,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:AH19"/>
+  <dimension ref="A1:AH20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -28657,7 +30194,7 @@
         <v>2000</v>
       </c>
       <c r="D3" s="19">
-        <f t="shared" ref="D3:D19" si="0">C3/B3</f>
+        <f t="shared" ref="D3:D20" si="0">C3/B3</f>
         <v>1939.8642095053349</v>
       </c>
       <c r="E3" s="19">
@@ -28665,7 +30202,7 @@
         <v>1939.8642095053349</v>
       </c>
       <c r="F3" s="19">
-        <f t="shared" ref="F3:F19" si="1">E3*B3</f>
+        <f t="shared" ref="F3:F20" si="1">E3*B3</f>
         <v>2000</v>
       </c>
       <c r="G3" s="19">
@@ -28673,11 +30210,11 @@
         <v>2000</v>
       </c>
       <c r="H3" s="19">
-        <f t="shared" ref="H3:H19" si="2">F3</f>
+        <f t="shared" ref="H3:H20" si="2">F3</f>
         <v>2000</v>
       </c>
       <c r="I3" s="19">
-        <f t="shared" ref="I3:I19" si="3">H3-G3</f>
+        <f t="shared" ref="I3:I20" si="3">H3-G3</f>
         <v>0</v>
       </c>
       <c r="J3" s="7"/>
@@ -28729,7 +30266,7 @@
         <v>2982.1073558648113</v>
       </c>
       <c r="E4" s="19">
-        <f t="shared" ref="E4:E19" si="4">E3+D4</f>
+        <f t="shared" ref="E4:E20" si="4">E3+D4</f>
         <v>4921.971565370146</v>
       </c>
       <c r="F4" s="19">
@@ -28737,7 +30274,7 @@
         <v>4951.503394762367</v>
       </c>
       <c r="G4" s="19">
-        <f t="shared" ref="G4:G19" si="5">G3+C4</f>
+        <f t="shared" ref="G4:G20" si="5">G3+C4</f>
         <v>5000</v>
       </c>
       <c r="H4" s="19">
@@ -28814,7 +30351,7 @@
         <v>0.96599999999999997</v>
       </c>
       <c r="C5" s="18">
-        <f t="shared" ref="C5:C19" si="7">IF(N5&lt;20,3000,2000)</f>
+        <f t="shared" ref="C5:C20" si="7">IF(N5&lt;20,3000,2000)</f>
         <v>3000</v>
       </c>
       <c r="D5" s="19">
@@ -28842,23 +30379,23 @@
         <v>-245.37546785243921</v>
       </c>
       <c r="J5" s="7">
-        <f t="shared" ref="J5:J19" si="8">MAX((B5-B4),0)</f>
+        <f t="shared" ref="J5:J20" si="8">MAX((B5-B4),0)</f>
         <v>0</v>
       </c>
       <c r="K5" s="7">
-        <f t="shared" ref="K5:K19" si="9">(K4*5+J5)/6</f>
+        <f t="shared" ref="K5:K20" si="9">(K4*5+J5)/6</f>
         <v>0</v>
       </c>
       <c r="L5" s="7">
-        <f t="shared" ref="L5:L19" si="10">ABS(B5-B4)</f>
+        <f t="shared" ref="L5:L20" si="10">ABS(B5-B4)</f>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="M5" s="7">
-        <f t="shared" ref="M5:M19" si="11">(M4*5+L5)/6</f>
+        <f t="shared" ref="M5:M20" si="11">(M4*5+L5)/6</f>
         <v>2.7499999999999931E-2</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" ref="N5:N19" si="12">K5*100/M5</f>
+        <f t="shared" ref="N5:N20" si="12">K5*100/M5</f>
         <v>0</v>
       </c>
       <c r="Z5" s="7"/>
@@ -29684,6 +31221,63 @@
         <v>23.977388204158451</v>
       </c>
     </row>
+    <row r="20" spans="1:14" ht="12.75">
+      <c r="A20" s="16">
+        <v>44895</v>
+      </c>
+      <c r="B20" s="17">
+        <f>VLOOKUP(A20,[1]HwabaoWP_szse_innovation_100!$A:$E,5)</f>
+        <v>0.72000002861022949</v>
+      </c>
+      <c r="C20" s="18">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+      <c r="D20" s="19">
+        <f t="shared" si="0"/>
+        <v>2777.7776673988105</v>
+      </c>
+      <c r="E20" s="19">
+        <f t="shared" si="4"/>
+        <v>51943.216935522461</v>
+      </c>
+      <c r="F20" s="19">
+        <f t="shared" si="1"/>
+        <v>37399.117679683528</v>
+      </c>
+      <c r="G20" s="19">
+        <f t="shared" si="5"/>
+        <v>44000</v>
+      </c>
+      <c r="H20" s="19">
+        <f t="shared" si="2"/>
+        <v>37399.117679683528</v>
+      </c>
+      <c r="I20" s="19">
+        <f t="shared" si="3"/>
+        <v>-6600.882320316472</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="8"/>
+        <v>3.3000051975250244E-2</v>
+      </c>
+      <c r="K20" s="7">
+        <f t="shared" si="9"/>
+        <v>1.4461814163367781E-2</v>
+      </c>
+      <c r="L20" s="7">
+        <f t="shared" si="10"/>
+        <v>3.3000051975250244E-2</v>
+      </c>
+      <c r="M20" s="7">
+        <f t="shared" si="11"/>
+        <v>4.287607908572403E-2</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="12"/>
+        <v>33.729329900837342</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -29695,9 +31289,9 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AH19"/>
+  <dimension ref="A1:AH20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -29812,7 +31406,7 @@
         <v>2000</v>
       </c>
       <c r="D3" s="19">
-        <f t="shared" ref="D3:D19" ca="1" si="0">C3/B3</f>
+        <f t="shared" ref="D3:D20" ca="1" si="0">C3/B3</f>
         <v>1939.8642095053349</v>
       </c>
       <c r="E3" s="19">
@@ -29820,7 +31414,7 @@
         <v>1939.8642095053349</v>
       </c>
       <c r="F3" s="19">
-        <f t="shared" ref="F3:F19" ca="1" si="1">E3*B3</f>
+        <f t="shared" ref="F3:F20" ca="1" si="1">E3*B3</f>
         <v>2000</v>
       </c>
       <c r="G3" s="19">
@@ -29828,11 +31422,11 @@
         <v>2000</v>
       </c>
       <c r="H3" s="19">
-        <f t="shared" ref="H3:H19" ca="1" si="2">F3</f>
+        <f t="shared" ref="H3:H20" ca="1" si="2">F3</f>
         <v>2000</v>
       </c>
       <c r="I3" s="19">
-        <f t="shared" ref="I3:I19" ca="1" si="3">H3-G3</f>
+        <f t="shared" ref="I3:I20" ca="1" si="3">H3-G3</f>
         <v>0</v>
       </c>
       <c r="J3" s="7">
@@ -29907,7 +31501,7 @@
         <v>1.006</v>
       </c>
       <c r="C4" s="18">
-        <f t="shared" ref="C4:C19" ca="1" si="4">IF(Q4&lt;0,3000,2000)</f>
+        <f t="shared" ref="C4:C20" ca="1" si="4">IF(Q4&lt;0,3000,2000)</f>
         <v>2000</v>
       </c>
       <c r="D4" s="19">
@@ -29915,7 +31509,7 @@
         <v>1988.0715705765408</v>
       </c>
       <c r="E4" s="19">
-        <f t="shared" ref="E4:E19" ca="1" si="5">E3+D4</f>
+        <f t="shared" ref="E4:E20" ca="1" si="5">E3+D4</f>
         <v>3927.9357800818757</v>
       </c>
       <c r="F4" s="19">
@@ -29923,7 +31517,7 @@
         <v>3951.503394762367</v>
       </c>
       <c r="G4" s="19">
-        <f t="shared" ref="G4:G19" ca="1" si="6">G3+C4</f>
+        <f t="shared" ref="G4:G20" ca="1" si="6">G3+C4</f>
         <v>4000</v>
       </c>
       <c r="H4" s="19">
@@ -29951,7 +31545,7 @@
         <v>0.94</v>
       </c>
       <c r="N4" s="7">
-        <f t="shared" ref="N4:N19" ca="1" si="7">(B4-M4)*100/(L4-M4)</f>
+        <f t="shared" ref="N4:N20" ca="1" si="7">(B4-M4)*100/(L4-M4)</f>
         <v>57.89473684210526</v>
       </c>
       <c r="O4" s="7">
@@ -29963,7 +31557,7 @@
         <v>83.200425305688029</v>
       </c>
       <c r="Q4" s="1">
-        <f t="shared" ref="Q4:Q19" ca="1" si="8">3*O4-2*P4</f>
+        <f t="shared" ref="Q4:Q20" ca="1" si="8">3*O4-2*P4</f>
         <v>64.221158958000927</v>
       </c>
       <c r="R4" s="21">
@@ -30060,11 +31654,11 @@
         <v>22.807017543859651</v>
       </c>
       <c r="O5" s="7">
-        <f t="shared" ref="O5:O19" ca="1" si="10">(N5+2*O4)/3</f>
+        <f t="shared" ref="O5:O20" ca="1" si="10">(N5+2*O4)/3</f>
         <v>58.851674641148101</v>
       </c>
       <c r="P5" s="7">
-        <f t="shared" ref="P5:P19" ca="1" si="11">(O5+2*P4)/3</f>
+        <f t="shared" ref="P5:P20" ca="1" si="11">(O5+2*P4)/3</f>
         <v>75.084175084174717</v>
       </c>
       <c r="Q5" s="1">
@@ -30554,11 +32148,11 @@
         <v>0.75</v>
       </c>
       <c r="L12" s="7">
-        <f t="shared" ref="L12:L19" ca="1" si="12">MAX(J4:J12)</f>
+        <f t="shared" ref="L12:L20" ca="1" si="12">MAX(J4:J12)</f>
         <v>1.054</v>
       </c>
       <c r="M12" s="7">
-        <f t="shared" ref="M12:M19" ca="1" si="13">MIN(K4:K12)</f>
+        <f t="shared" ref="M12:M20" ca="1" si="13">MIN(K4:K12)</f>
         <v>0.75</v>
       </c>
       <c r="N12" s="7">
@@ -31060,6 +32654,75 @@
       <c r="Q19" s="1">
         <f t="shared" ca="1" si="8"/>
         <v>10.691805251451996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="12.75">
+      <c r="A20" s="16">
+        <v>44895</v>
+      </c>
+      <c r="B20" s="17">
+        <f>VLOOKUP(A20,[1]HwabaoWP_szse_innovation_100!$A:$E,5)</f>
+        <v>0.72000002861022949</v>
+      </c>
+      <c r="C20" s="18">
+        <f t="shared" ca="1" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="D20" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2777.7776673988105</v>
+      </c>
+      <c r="E20" s="19">
+        <f t="shared" ca="1" si="5"/>
+        <v>43887.771693479837</v>
+      </c>
+      <c r="F20" s="19">
+        <f t="shared" ca="1" si="1"/>
+        <v>31599.196874944704</v>
+      </c>
+      <c r="G20" s="19">
+        <f t="shared" ca="1" si="6"/>
+        <v>37000</v>
+      </c>
+      <c r="H20" s="19">
+        <f t="shared" ca="1" si="2"/>
+        <v>31599.196874944704</v>
+      </c>
+      <c r="I20" s="19">
+        <f t="shared" ca="1" si="3"/>
+        <v>-5400.8031250552958</v>
+      </c>
+      <c r="J20" s="7">
+        <f ca="1">MAX(VLOOKUP(A20,[1]HwabaoWP_szse_innovation_100!$A:$C,3),OFFSET([1]HwabaoWP_szse_innovation_100!$N$1,(MATCH(A20,[1]HwabaoWP_szse_innovation_100!$A:$A)-2),))</f>
+        <v>0.74500000476837158</v>
+      </c>
+      <c r="K20" s="7">
+        <f ca="1">MIN(VLOOKUP(A20,[1]HwabaoWP_szse_innovation_100!$A:$D,4),OFFSET([1]HwabaoWP_szse_innovation_100!$O$1,(MATCH(A20,[1]HwabaoWP_szse_innovation_100!$A:$A)-2),))</f>
+        <v>0.68400001525878906</v>
+      </c>
+      <c r="L20" s="7">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.88599997758865356</v>
+      </c>
+      <c r="M20" s="7">
+        <f t="shared" ca="1" si="13"/>
+        <v>0.65399998426437378</v>
+      </c>
+      <c r="N20" s="7">
+        <f t="shared" ca="1" si="7"/>
+        <v>28.448295795251873</v>
+      </c>
+      <c r="O20" s="7">
+        <f t="shared" ca="1" si="10"/>
+        <v>23.752534975058655</v>
+      </c>
+      <c r="P20" s="7">
+        <f t="shared" ca="1" si="11"/>
+        <v>25.758231139497596</v>
+      </c>
+      <c r="Q20" s="1">
+        <f t="shared" ca="1" si="8"/>
+        <v>19.741142646180776</v>
       </c>
     </row>
   </sheetData>
@@ -31073,9 +32736,9 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:AC19"/>
+  <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -31174,7 +32837,7 @@
         <v>2000</v>
       </c>
       <c r="E3" s="19">
-        <f t="shared" ref="E3:E19" si="0">D3/B3</f>
+        <f t="shared" ref="E3:E20" si="0">D3/B3</f>
         <v>1939.8642095053349</v>
       </c>
       <c r="F3" s="19">
@@ -31182,7 +32845,7 @@
         <v>1939.8642095053349</v>
       </c>
       <c r="G3" s="19">
-        <f t="shared" ref="G3:G19" si="1">F3*B3</f>
+        <f t="shared" ref="G3:G20" si="1">F3*B3</f>
         <v>2000</v>
       </c>
       <c r="H3" s="19">
@@ -31190,11 +32853,11 @@
         <v>2000</v>
       </c>
       <c r="I3" s="19">
-        <f t="shared" ref="I3:I19" si="2">G3</f>
+        <f t="shared" ref="I3:I20" si="2">G3</f>
         <v>2000</v>
       </c>
       <c r="J3" s="19">
-        <f t="shared" ref="J3:J19" si="3">I3-H3</f>
+        <f t="shared" ref="J3:J20" si="3">I3-H3</f>
         <v>0</v>
       </c>
       <c r="K3" s="7"/>
@@ -31242,7 +32905,7 @@
         <v>39.930000305175781</v>
       </c>
       <c r="D4" s="18">
-        <f t="shared" ref="D4:D19" si="4">D3</f>
+        <f t="shared" ref="D4:D20" si="4">D3</f>
         <v>2000</v>
       </c>
       <c r="E4" s="19">
@@ -31250,7 +32913,7 @@
         <v>1988.0715705765408</v>
       </c>
       <c r="F4" s="19">
-        <f t="shared" ref="F4:F19" si="5">F3+E4</f>
+        <f t="shared" ref="F4:F20" si="5">F3+E4</f>
         <v>3927.9357800818757</v>
       </c>
       <c r="G4" s="19">
@@ -31258,7 +32921,7 @@
         <v>3951.503394762367</v>
       </c>
       <c r="H4" s="19">
-        <f t="shared" ref="H4:H19" si="6">H3+D4</f>
+        <f t="shared" ref="H4:H20" si="6">H3+D4</f>
         <v>4000</v>
       </c>
       <c r="I4" s="19">
@@ -31960,6 +33623,47 @@
         <v>-6624.8592822413775</v>
       </c>
     </row>
+    <row r="20" spans="1:11" ht="12.75">
+      <c r="A20" s="16">
+        <v>44895</v>
+      </c>
+      <c r="B20" s="17">
+        <f>VLOOKUP(A20,[1]HwabaoWP_szse_innovation_100!$A:$E,5)</f>
+        <v>0.72000002861022949</v>
+      </c>
+      <c r="C20" s="17">
+        <f>VLOOKUP(A20,[2]myPEPB!$B:$C,2)</f>
+        <v>22.809999470000001</v>
+      </c>
+      <c r="D20" s="18">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="E20" s="19">
+        <f t="shared" si="0"/>
+        <v>2777.7776673988105</v>
+      </c>
+      <c r="F20" s="19">
+        <f t="shared" si="5"/>
+        <v>42625.145424011906</v>
+      </c>
+      <c r="G20" s="19">
+        <f t="shared" si="1"/>
+        <v>30690.105924803764</v>
+      </c>
+      <c r="H20" s="19">
+        <f t="shared" si="6"/>
+        <v>36000</v>
+      </c>
+      <c r="I20" s="19">
+        <f t="shared" si="2"/>
+        <v>30690.105924803764</v>
+      </c>
+      <c r="J20" s="19">
+        <f t="shared" si="3"/>
+        <v>-5309.8940751962364</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J2"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>